<commit_message>
added visible current tact+fixed double legend item
</commit_message>
<xml_diff>
--- a/imgs/0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand.xlsx
+++ b/imgs/0_5_T1_SP_GRU_EG0_3101_03_F-P-001 - Wand.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L393"/>
+  <dimension ref="A1:N408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,16 @@
           <t>Sonst.</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Mauerwerk@Mauern</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Mauerwerk@Erledigt</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -520,6 +530,8 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -546,6 +558,8 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -572,6 +586,8 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -598,6 +614,8 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -624,6 +642,8 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -650,6 +670,8 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -676,6 +698,8 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -702,6 +726,8 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -728,6 +754,8 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -754,6 +782,8 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -780,6 +810,8 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -806,6 +838,8 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -832,6 +866,8 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -858,6 +894,8 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -884,6 +922,8 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -910,6 +950,8 @@
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -936,6 +978,8 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -962,6 +1006,8 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -988,6 +1034,8 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1014,6 +1062,8 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1040,6 +1090,8 @@
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1066,6 +1118,8 @@
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1092,6 +1146,8 @@
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1118,6 +1174,8 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1144,6 +1202,8 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1170,6 +1230,8 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1196,6 +1258,8 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1222,6 +1286,8 @@
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1248,6 +1314,8 @@
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1274,6 +1342,8 @@
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1300,6 +1370,8 @@
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1326,6 +1398,8 @@
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1352,6 +1426,8 @@
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1378,6 +1454,8 @@
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1404,6 +1482,8 @@
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1430,6 +1510,8 @@
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1456,6 +1538,8 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1482,6 +1566,8 @@
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1508,6 +1594,8 @@
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1534,6 +1622,8 @@
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1560,6 +1650,8 @@
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1586,6 +1678,8 @@
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1612,6 +1706,8 @@
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1638,6 +1734,8 @@
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1664,6 +1762,8 @@
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1690,6 +1790,8 @@
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1716,6 +1818,8 @@
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1742,6 +1846,8 @@
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1768,6 +1874,8 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1794,6 +1902,8 @@
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1820,6 +1930,8 @@
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1846,6 +1958,8 @@
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1872,6 +1986,8 @@
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1898,6 +2014,8 @@
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1924,6 +2042,8 @@
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1950,6 +2070,8 @@
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1976,6 +2098,8 @@
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2002,6 +2126,8 @@
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2028,6 +2154,8 @@
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2054,6 +2182,8 @@
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2080,6 +2210,8 @@
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2106,6 +2238,8 @@
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2132,6 +2266,8 @@
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2158,6 +2294,8 @@
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2184,6 +2322,8 @@
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2210,6 +2350,8 @@
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2236,6 +2378,8 @@
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2262,6 +2406,8 @@
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2288,6 +2434,8 @@
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2314,6 +2462,8 @@
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2340,6 +2490,8 @@
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2366,6 +2518,8 @@
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2392,6 +2546,8 @@
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2418,6 +2574,8 @@
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2444,6 +2602,8 @@
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2470,6 +2630,8 @@
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2496,6 +2658,8 @@
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2522,6 +2686,8 @@
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2548,6 +2714,8 @@
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2574,6 +2742,8 @@
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2600,6 +2770,8 @@
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2626,6 +2798,8 @@
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2652,6 +2826,8 @@
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2678,6 +2854,8 @@
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2704,6 +2882,8 @@
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2730,6 +2910,8 @@
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2756,6 +2938,8 @@
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2782,6 +2966,8 @@
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2808,6 +2994,8 @@
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2834,6 +3022,8 @@
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2860,6 +3050,8 @@
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2886,6 +3078,8 @@
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2912,6 +3106,8 @@
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2938,6 +3134,8 @@
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2964,6 +3162,8 @@
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2990,6 +3190,8 @@
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3016,6 +3218,8 @@
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3042,6 +3246,8 @@
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3068,6 +3274,8 @@
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3094,6 +3302,8 @@
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3120,6 +3330,8 @@
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3146,6 +3358,8 @@
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3172,6 +3386,8 @@
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3198,6 +3414,8 @@
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3224,6 +3442,8 @@
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3250,6 +3470,8 @@
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3276,6 +3498,8 @@
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3302,6 +3526,8 @@
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3328,6 +3554,8 @@
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3354,6 +3582,8 @@
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3380,6 +3610,8 @@
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3406,6 +3638,8 @@
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3432,6 +3666,8 @@
       <c r="J114" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3458,6 +3694,8 @@
       <c r="J115" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3484,6 +3722,8 @@
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3510,6 +3750,8 @@
       <c r="J117" t="inlineStr"/>
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3536,6 +3778,8 @@
       <c r="J118" t="inlineStr"/>
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3562,6 +3806,8 @@
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3588,6 +3834,8 @@
       <c r="J120" t="inlineStr"/>
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3614,6 +3862,8 @@
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3640,6 +3890,8 @@
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3666,6 +3918,8 @@
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3692,6 +3946,8 @@
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3718,6 +3974,8 @@
       <c r="J125" t="inlineStr"/>
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr"/>
+      <c r="M125" t="inlineStr"/>
+      <c r="N125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3744,6 +4002,8 @@
       <c r="J126" t="inlineStr"/>
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3770,6 +4030,8 @@
       <c r="J127" t="inlineStr"/>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3796,6 +4058,8 @@
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr"/>
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3822,6 +4086,8 @@
       <c r="J129" t="inlineStr"/>
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3848,6 +4114,8 @@
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3874,6 +4142,8 @@
       <c r="J131" t="inlineStr"/>
       <c r="K131" t="inlineStr"/>
       <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3900,6 +4170,8 @@
       <c r="J132" t="inlineStr"/>
       <c r="K132" t="inlineStr"/>
       <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3926,6 +4198,8 @@
       <c r="J133" t="inlineStr"/>
       <c r="K133" t="inlineStr"/>
       <c r="L133" t="inlineStr"/>
+      <c r="M133" t="inlineStr"/>
+      <c r="N133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3952,6 +4226,8 @@
       <c r="J134" t="inlineStr"/>
       <c r="K134" t="inlineStr"/>
       <c r="L134" t="inlineStr"/>
+      <c r="M134" t="inlineStr"/>
+      <c r="N134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3978,6 +4254,8 @@
       <c r="J135" t="inlineStr"/>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr"/>
+      <c r="M135" t="inlineStr"/>
+      <c r="N135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4004,6 +4282,8 @@
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr"/>
+      <c r="M136" t="inlineStr"/>
+      <c r="N136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4030,6 +4310,8 @@
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4056,6 +4338,8 @@
       <c r="J138" t="inlineStr"/>
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4082,6 +4366,8 @@
       <c r="J139" t="inlineStr"/>
       <c r="K139" t="inlineStr"/>
       <c r="L139" t="inlineStr"/>
+      <c r="M139" t="inlineStr"/>
+      <c r="N139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4108,6 +4394,8 @@
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr"/>
+      <c r="M140" t="inlineStr"/>
+      <c r="N140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -4134,6 +4422,8 @@
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
+      <c r="N141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4160,6 +4450,8 @@
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr"/>
+      <c r="M142" t="inlineStr"/>
+      <c r="N142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4186,6 +4478,8 @@
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
+      <c r="N143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4212,6 +4506,8 @@
       <c r="J144" t="inlineStr"/>
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr"/>
+      <c r="M144" t="inlineStr"/>
+      <c r="N144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -4238,6 +4534,8 @@
       <c r="J145" t="inlineStr"/>
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr"/>
+      <c r="M145" t="inlineStr"/>
+      <c r="N145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4264,6 +4562,8 @@
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="inlineStr"/>
       <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -4290,6 +4590,8 @@
       <c r="J147" t="inlineStr"/>
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr"/>
+      <c r="M147" t="inlineStr"/>
+      <c r="N147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -4316,6 +4618,8 @@
       <c r="J148" t="inlineStr"/>
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
+      <c r="N148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -4342,6 +4646,8 @@
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr"/>
+      <c r="M149" t="inlineStr"/>
+      <c r="N149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -4368,6 +4674,8 @@
       <c r="J150" t="inlineStr"/>
       <c r="K150" t="inlineStr"/>
       <c r="L150" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
+      <c r="N150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -4422,6 +4730,8 @@
         </is>
       </c>
       <c r="L151" t="inlineStr"/>
+      <c r="M151" t="inlineStr"/>
+      <c r="N151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -4476,6 +4786,8 @@
         </is>
       </c>
       <c r="L152" t="inlineStr"/>
+      <c r="M152" t="inlineStr"/>
+      <c r="N152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -4530,6 +4842,8 @@
         </is>
       </c>
       <c r="L153" t="inlineStr"/>
+      <c r="M153" t="inlineStr"/>
+      <c r="N153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -4584,6 +4898,8 @@
         </is>
       </c>
       <c r="L154" t="inlineStr"/>
+      <c r="M154" t="inlineStr"/>
+      <c r="N154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -4638,6 +4954,8 @@
         </is>
       </c>
       <c r="L155" t="inlineStr"/>
+      <c r="M155" t="inlineStr"/>
+      <c r="N155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -4692,6 +5010,8 @@
         </is>
       </c>
       <c r="L156" t="inlineStr"/>
+      <c r="M156" t="inlineStr"/>
+      <c r="N156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -4746,6 +5066,8 @@
         </is>
       </c>
       <c r="L157" t="inlineStr"/>
+      <c r="M157" t="inlineStr"/>
+      <c r="N157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -4772,6 +5094,8 @@
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="inlineStr"/>
       <c r="L158" t="inlineStr"/>
+      <c r="M158" t="inlineStr"/>
+      <c r="N158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -4798,6 +5122,8 @@
       <c r="J159" t="inlineStr"/>
       <c r="K159" t="inlineStr"/>
       <c r="L159" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
+      <c r="N159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -4824,6 +5150,8 @@
       <c r="J160" t="inlineStr"/>
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
+      <c r="N160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -4850,6 +5178,8 @@
       <c r="J161" t="inlineStr"/>
       <c r="K161" t="inlineStr"/>
       <c r="L161" t="inlineStr"/>
+      <c r="M161" t="inlineStr"/>
+      <c r="N161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -4876,6 +5206,8 @@
       <c r="J162" t="inlineStr"/>
       <c r="K162" t="inlineStr"/>
       <c r="L162" t="inlineStr"/>
+      <c r="M162" t="inlineStr"/>
+      <c r="N162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -4902,6 +5234,8 @@
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="inlineStr"/>
       <c r="L163" t="inlineStr"/>
+      <c r="M163" t="inlineStr"/>
+      <c r="N163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -4928,6 +5262,8 @@
       <c r="J164" t="inlineStr"/>
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr"/>
+      <c r="M164" t="inlineStr"/>
+      <c r="N164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -4982,6 +5318,8 @@
         </is>
       </c>
       <c r="L165" t="inlineStr"/>
+      <c r="M165" t="inlineStr"/>
+      <c r="N165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -5036,6 +5374,8 @@
         </is>
       </c>
       <c r="L166" t="inlineStr"/>
+      <c r="M166" t="inlineStr"/>
+      <c r="N166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -5090,6 +5430,8 @@
         </is>
       </c>
       <c r="L167" t="inlineStr"/>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -5144,6 +5486,8 @@
         </is>
       </c>
       <c r="L168" t="inlineStr"/>
+      <c r="M168" t="inlineStr"/>
+      <c r="N168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -5198,6 +5542,8 @@
         </is>
       </c>
       <c r="L169" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -5252,6 +5598,8 @@
         </is>
       </c>
       <c r="L170" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -5306,6 +5654,8 @@
         </is>
       </c>
       <c r="L171" t="inlineStr"/>
+      <c r="M171" t="inlineStr"/>
+      <c r="N171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -5360,6 +5710,8 @@
         </is>
       </c>
       <c r="L172" t="inlineStr"/>
+      <c r="M172" t="inlineStr"/>
+      <c r="N172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -5414,6 +5766,8 @@
         </is>
       </c>
       <c r="L173" t="inlineStr"/>
+      <c r="M173" t="inlineStr"/>
+      <c r="N173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -5468,6 +5822,8 @@
         </is>
       </c>
       <c r="L174" t="inlineStr"/>
+      <c r="M174" t="inlineStr"/>
+      <c r="N174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -5522,6 +5878,8 @@
         </is>
       </c>
       <c r="L175" t="inlineStr"/>
+      <c r="M175" t="inlineStr"/>
+      <c r="N175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -5576,6 +5934,8 @@
         </is>
       </c>
       <c r="L176" t="inlineStr"/>
+      <c r="M176" t="inlineStr"/>
+      <c r="N176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -5630,6 +5990,8 @@
         </is>
       </c>
       <c r="L177" t="inlineStr"/>
+      <c r="M177" t="inlineStr"/>
+      <c r="N177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -5684,6 +6046,8 @@
         </is>
       </c>
       <c r="L178" t="inlineStr"/>
+      <c r="M178" t="inlineStr"/>
+      <c r="N178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -5738,6 +6102,8 @@
         </is>
       </c>
       <c r="L179" t="inlineStr"/>
+      <c r="M179" t="inlineStr"/>
+      <c r="N179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -5792,6 +6158,8 @@
         </is>
       </c>
       <c r="L180" t="inlineStr"/>
+      <c r="M180" t="inlineStr"/>
+      <c r="N180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -5846,6 +6214,8 @@
         </is>
       </c>
       <c r="L181" t="inlineStr"/>
+      <c r="M181" t="inlineStr"/>
+      <c r="N181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -5900,6 +6270,8 @@
         </is>
       </c>
       <c r="L182" t="inlineStr"/>
+      <c r="M182" t="inlineStr"/>
+      <c r="N182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -5926,6 +6298,8 @@
       <c r="J183" t="inlineStr"/>
       <c r="K183" t="inlineStr"/>
       <c r="L183" t="inlineStr"/>
+      <c r="M183" t="inlineStr"/>
+      <c r="N183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -5952,6 +6326,8 @@
       <c r="J184" t="inlineStr"/>
       <c r="K184" t="inlineStr"/>
       <c r="L184" t="inlineStr"/>
+      <c r="M184" t="inlineStr"/>
+      <c r="N184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -5978,6 +6354,8 @@
       <c r="J185" t="inlineStr"/>
       <c r="K185" t="inlineStr"/>
       <c r="L185" t="inlineStr"/>
+      <c r="M185" t="inlineStr"/>
+      <c r="N185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -6004,6 +6382,8 @@
       <c r="J186" t="inlineStr"/>
       <c r="K186" t="inlineStr"/>
       <c r="L186" t="inlineStr"/>
+      <c r="M186" t="inlineStr"/>
+      <c r="N186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -6030,6 +6410,8 @@
       <c r="J187" t="inlineStr"/>
       <c r="K187" t="inlineStr"/>
       <c r="L187" t="inlineStr"/>
+      <c r="M187" t="inlineStr"/>
+      <c r="N187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -6056,6 +6438,8 @@
       <c r="J188" t="inlineStr"/>
       <c r="K188" t="inlineStr"/>
       <c r="L188" t="inlineStr"/>
+      <c r="M188" t="inlineStr"/>
+      <c r="N188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -6082,6 +6466,8 @@
       <c r="J189" t="inlineStr"/>
       <c r="K189" t="inlineStr"/>
       <c r="L189" t="inlineStr"/>
+      <c r="M189" t="inlineStr"/>
+      <c r="N189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -6108,6 +6494,8 @@
       <c r="J190" t="inlineStr"/>
       <c r="K190" t="inlineStr"/>
       <c r="L190" t="inlineStr"/>
+      <c r="M190" t="inlineStr"/>
+      <c r="N190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -6134,6 +6522,8 @@
       <c r="J191" t="inlineStr"/>
       <c r="K191" t="inlineStr"/>
       <c r="L191" t="inlineStr"/>
+      <c r="M191" t="inlineStr"/>
+      <c r="N191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -6160,6 +6550,8 @@
       <c r="J192" t="inlineStr"/>
       <c r="K192" t="inlineStr"/>
       <c r="L192" t="inlineStr"/>
+      <c r="M192" t="inlineStr"/>
+      <c r="N192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -6186,6 +6578,8 @@
       <c r="J193" t="inlineStr"/>
       <c r="K193" t="inlineStr"/>
       <c r="L193" t="inlineStr"/>
+      <c r="M193" t="inlineStr"/>
+      <c r="N193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -6212,6 +6606,8 @@
       <c r="J194" t="inlineStr"/>
       <c r="K194" t="inlineStr"/>
       <c r="L194" t="inlineStr"/>
+      <c r="M194" t="inlineStr"/>
+      <c r="N194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -6238,6 +6634,8 @@
       <c r="J195" t="inlineStr"/>
       <c r="K195" t="inlineStr"/>
       <c r="L195" t="inlineStr"/>
+      <c r="M195" t="inlineStr"/>
+      <c r="N195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -6264,6 +6662,8 @@
       <c r="J196" t="inlineStr"/>
       <c r="K196" t="inlineStr"/>
       <c r="L196" t="inlineStr"/>
+      <c r="M196" t="inlineStr"/>
+      <c r="N196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -6290,6 +6690,8 @@
       <c r="J197" t="inlineStr"/>
       <c r="K197" t="inlineStr"/>
       <c r="L197" t="inlineStr"/>
+      <c r="M197" t="inlineStr"/>
+      <c r="N197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -6316,6 +6718,8 @@
       <c r="J198" t="inlineStr"/>
       <c r="K198" t="inlineStr"/>
       <c r="L198" t="inlineStr"/>
+      <c r="M198" t="inlineStr"/>
+      <c r="N198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -6342,6 +6746,8 @@
       <c r="J199" t="inlineStr"/>
       <c r="K199" t="inlineStr"/>
       <c r="L199" t="inlineStr"/>
+      <c r="M199" t="inlineStr"/>
+      <c r="N199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -6368,6 +6774,8 @@
       <c r="J200" t="inlineStr"/>
       <c r="K200" t="inlineStr"/>
       <c r="L200" t="inlineStr"/>
+      <c r="M200" t="inlineStr"/>
+      <c r="N200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -6394,6 +6802,8 @@
       <c r="J201" t="inlineStr"/>
       <c r="K201" t="inlineStr"/>
       <c r="L201" t="inlineStr"/>
+      <c r="M201" t="inlineStr"/>
+      <c r="N201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -6420,6 +6830,8 @@
       <c r="J202" t="inlineStr"/>
       <c r="K202" t="inlineStr"/>
       <c r="L202" t="inlineStr"/>
+      <c r="M202" t="inlineStr"/>
+      <c r="N202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -6446,6 +6858,8 @@
       <c r="J203" t="inlineStr"/>
       <c r="K203" t="inlineStr"/>
       <c r="L203" t="inlineStr"/>
+      <c r="M203" t="inlineStr"/>
+      <c r="N203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -6472,6 +6886,8 @@
       <c r="J204" t="inlineStr"/>
       <c r="K204" t="inlineStr"/>
       <c r="L204" t="inlineStr"/>
+      <c r="M204" t="inlineStr"/>
+      <c r="N204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -6498,6 +6914,8 @@
       <c r="J205" t="inlineStr"/>
       <c r="K205" t="inlineStr"/>
       <c r="L205" t="inlineStr"/>
+      <c r="M205" t="inlineStr"/>
+      <c r="N205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -6524,6 +6942,8 @@
       <c r="J206" t="inlineStr"/>
       <c r="K206" t="inlineStr"/>
       <c r="L206" t="inlineStr"/>
+      <c r="M206" t="inlineStr"/>
+      <c r="N206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -6550,6 +6970,8 @@
       <c r="J207" t="inlineStr"/>
       <c r="K207" t="inlineStr"/>
       <c r="L207" t="inlineStr"/>
+      <c r="M207" t="inlineStr"/>
+      <c r="N207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -6576,6 +6998,8 @@
       <c r="J208" t="inlineStr"/>
       <c r="K208" t="inlineStr"/>
       <c r="L208" t="inlineStr"/>
+      <c r="M208" t="inlineStr"/>
+      <c r="N208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -6602,6 +7026,8 @@
       <c r="J209" t="inlineStr"/>
       <c r="K209" t="inlineStr"/>
       <c r="L209" t="inlineStr"/>
+      <c r="M209" t="inlineStr"/>
+      <c r="N209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -6628,6 +7054,8 @@
       <c r="J210" t="inlineStr"/>
       <c r="K210" t="inlineStr"/>
       <c r="L210" t="inlineStr"/>
+      <c r="M210" t="inlineStr"/>
+      <c r="N210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -6654,6 +7082,8 @@
       <c r="J211" t="inlineStr"/>
       <c r="K211" t="inlineStr"/>
       <c r="L211" t="inlineStr"/>
+      <c r="M211" t="inlineStr"/>
+      <c r="N211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -6680,6 +7110,8 @@
       <c r="J212" t="inlineStr"/>
       <c r="K212" t="inlineStr"/>
       <c r="L212" t="inlineStr"/>
+      <c r="M212" t="inlineStr"/>
+      <c r="N212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -6706,6 +7138,8 @@
       <c r="J213" t="inlineStr"/>
       <c r="K213" t="inlineStr"/>
       <c r="L213" t="inlineStr"/>
+      <c r="M213" t="inlineStr"/>
+      <c r="N213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -6732,6 +7166,8 @@
       <c r="J214" t="inlineStr"/>
       <c r="K214" t="inlineStr"/>
       <c r="L214" t="inlineStr"/>
+      <c r="M214" t="inlineStr"/>
+      <c r="N214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -6758,6 +7194,8 @@
       <c r="J215" t="inlineStr"/>
       <c r="K215" t="inlineStr"/>
       <c r="L215" t="inlineStr"/>
+      <c r="M215" t="inlineStr"/>
+      <c r="N215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -6784,6 +7222,8 @@
       <c r="J216" t="inlineStr"/>
       <c r="K216" t="inlineStr"/>
       <c r="L216" t="inlineStr"/>
+      <c r="M216" t="inlineStr"/>
+      <c r="N216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -6810,6 +7250,8 @@
       <c r="J217" t="inlineStr"/>
       <c r="K217" t="inlineStr"/>
       <c r="L217" t="inlineStr"/>
+      <c r="M217" t="inlineStr"/>
+      <c r="N217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -6836,6 +7278,8 @@
       <c r="J218" t="inlineStr"/>
       <c r="K218" t="inlineStr"/>
       <c r="L218" t="inlineStr"/>
+      <c r="M218" t="inlineStr"/>
+      <c r="N218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -6862,6 +7306,8 @@
       <c r="J219" t="inlineStr"/>
       <c r="K219" t="inlineStr"/>
       <c r="L219" t="inlineStr"/>
+      <c r="M219" t="inlineStr"/>
+      <c r="N219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -6888,6 +7334,8 @@
       <c r="J220" t="inlineStr"/>
       <c r="K220" t="inlineStr"/>
       <c r="L220" t="inlineStr"/>
+      <c r="M220" t="inlineStr"/>
+      <c r="N220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -6914,6 +7362,8 @@
       <c r="J221" t="inlineStr"/>
       <c r="K221" t="inlineStr"/>
       <c r="L221" t="inlineStr"/>
+      <c r="M221" t="inlineStr"/>
+      <c r="N221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -6940,6 +7390,8 @@
       <c r="J222" t="inlineStr"/>
       <c r="K222" t="inlineStr"/>
       <c r="L222" t="inlineStr"/>
+      <c r="M222" t="inlineStr"/>
+      <c r="N222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -6966,6 +7418,8 @@
       <c r="J223" t="inlineStr"/>
       <c r="K223" t="inlineStr"/>
       <c r="L223" t="inlineStr"/>
+      <c r="M223" t="inlineStr"/>
+      <c r="N223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -6992,6 +7446,8 @@
       <c r="J224" t="inlineStr"/>
       <c r="K224" t="inlineStr"/>
       <c r="L224" t="inlineStr"/>
+      <c r="M224" t="inlineStr"/>
+      <c r="N224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -7018,6 +7474,8 @@
       <c r="J225" t="inlineStr"/>
       <c r="K225" t="inlineStr"/>
       <c r="L225" t="inlineStr"/>
+      <c r="M225" t="inlineStr"/>
+      <c r="N225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -7044,6 +7502,8 @@
       <c r="J226" t="inlineStr"/>
       <c r="K226" t="inlineStr"/>
       <c r="L226" t="inlineStr"/>
+      <c r="M226" t="inlineStr"/>
+      <c r="N226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -7070,6 +7530,8 @@
       <c r="J227" t="inlineStr"/>
       <c r="K227" t="inlineStr"/>
       <c r="L227" t="inlineStr"/>
+      <c r="M227" t="inlineStr"/>
+      <c r="N227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -7096,6 +7558,8 @@
       <c r="J228" t="inlineStr"/>
       <c r="K228" t="inlineStr"/>
       <c r="L228" t="inlineStr"/>
+      <c r="M228" t="inlineStr"/>
+      <c r="N228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -7122,6 +7586,8 @@
       <c r="J229" t="inlineStr"/>
       <c r="K229" t="inlineStr"/>
       <c r="L229" t="inlineStr"/>
+      <c r="M229" t="inlineStr"/>
+      <c r="N229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -7148,6 +7614,8 @@
       <c r="J230" t="inlineStr"/>
       <c r="K230" t="inlineStr"/>
       <c r="L230" t="inlineStr"/>
+      <c r="M230" t="inlineStr"/>
+      <c r="N230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -7174,6 +7642,8 @@
       <c r="J231" t="inlineStr"/>
       <c r="K231" t="inlineStr"/>
       <c r="L231" t="inlineStr"/>
+      <c r="M231" t="inlineStr"/>
+      <c r="N231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -7200,6 +7670,8 @@
       <c r="J232" t="inlineStr"/>
       <c r="K232" t="inlineStr"/>
       <c r="L232" t="inlineStr"/>
+      <c r="M232" t="inlineStr"/>
+      <c r="N232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -7226,6 +7698,8 @@
       <c r="J233" t="inlineStr"/>
       <c r="K233" t="inlineStr"/>
       <c r="L233" t="inlineStr"/>
+      <c r="M233" t="inlineStr"/>
+      <c r="N233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -7252,6 +7726,8 @@
       <c r="J234" t="inlineStr"/>
       <c r="K234" t="inlineStr"/>
       <c r="L234" t="inlineStr"/>
+      <c r="M234" t="inlineStr"/>
+      <c r="N234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -7278,6 +7754,8 @@
       <c r="J235" t="inlineStr"/>
       <c r="K235" t="inlineStr"/>
       <c r="L235" t="inlineStr"/>
+      <c r="M235" t="inlineStr"/>
+      <c r="N235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -7304,6 +7782,8 @@
       <c r="J236" t="inlineStr"/>
       <c r="K236" t="inlineStr"/>
       <c r="L236" t="inlineStr"/>
+      <c r="M236" t="inlineStr"/>
+      <c r="N236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -7330,6 +7810,8 @@
       <c r="J237" t="inlineStr"/>
       <c r="K237" t="inlineStr"/>
       <c r="L237" t="inlineStr"/>
+      <c r="M237" t="inlineStr"/>
+      <c r="N237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -7356,6 +7838,8 @@
       <c r="J238" t="inlineStr"/>
       <c r="K238" t="inlineStr"/>
       <c r="L238" t="inlineStr"/>
+      <c r="M238" t="inlineStr"/>
+      <c r="N238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -7382,6 +7866,8 @@
       <c r="J239" t="inlineStr"/>
       <c r="K239" t="inlineStr"/>
       <c r="L239" t="inlineStr"/>
+      <c r="M239" t="inlineStr"/>
+      <c r="N239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -7408,6 +7894,8 @@
       <c r="J240" t="inlineStr"/>
       <c r="K240" t="inlineStr"/>
       <c r="L240" t="inlineStr"/>
+      <c r="M240" t="inlineStr"/>
+      <c r="N240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -7434,6 +7922,8 @@
       <c r="J241" t="inlineStr"/>
       <c r="K241" t="inlineStr"/>
       <c r="L241" t="inlineStr"/>
+      <c r="M241" t="inlineStr"/>
+      <c r="N241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -7460,6 +7950,8 @@
       <c r="J242" t="inlineStr"/>
       <c r="K242" t="inlineStr"/>
       <c r="L242" t="inlineStr"/>
+      <c r="M242" t="inlineStr"/>
+      <c r="N242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -7486,6 +7978,8 @@
       <c r="J243" t="inlineStr"/>
       <c r="K243" t="inlineStr"/>
       <c r="L243" t="inlineStr"/>
+      <c r="M243" t="inlineStr"/>
+      <c r="N243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -7512,6 +8006,8 @@
       <c r="J244" t="inlineStr"/>
       <c r="K244" t="inlineStr"/>
       <c r="L244" t="inlineStr"/>
+      <c r="M244" t="inlineStr"/>
+      <c r="N244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -7538,6 +8034,8 @@
       <c r="J245" t="inlineStr"/>
       <c r="K245" t="inlineStr"/>
       <c r="L245" t="inlineStr"/>
+      <c r="M245" t="inlineStr"/>
+      <c r="N245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -7564,6 +8062,8 @@
       <c r="J246" t="inlineStr"/>
       <c r="K246" t="inlineStr"/>
       <c r="L246" t="inlineStr"/>
+      <c r="M246" t="inlineStr"/>
+      <c r="N246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -7590,6 +8090,8 @@
       <c r="J247" t="inlineStr"/>
       <c r="K247" t="inlineStr"/>
       <c r="L247" t="inlineStr"/>
+      <c r="M247" t="inlineStr"/>
+      <c r="N247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -7616,6 +8118,8 @@
       <c r="J248" t="inlineStr"/>
       <c r="K248" t="inlineStr"/>
       <c r="L248" t="inlineStr"/>
+      <c r="M248" t="inlineStr"/>
+      <c r="N248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -7642,6 +8146,8 @@
       <c r="J249" t="inlineStr"/>
       <c r="K249" t="inlineStr"/>
       <c r="L249" t="inlineStr"/>
+      <c r="M249" t="inlineStr"/>
+      <c r="N249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -7668,6 +8174,8 @@
       <c r="J250" t="inlineStr"/>
       <c r="K250" t="inlineStr"/>
       <c r="L250" t="inlineStr"/>
+      <c r="M250" t="inlineStr"/>
+      <c r="N250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -7694,6 +8202,8 @@
       <c r="J251" t="inlineStr"/>
       <c r="K251" t="inlineStr"/>
       <c r="L251" t="inlineStr"/>
+      <c r="M251" t="inlineStr"/>
+      <c r="N251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -7720,6 +8230,8 @@
       <c r="J252" t="inlineStr"/>
       <c r="K252" t="inlineStr"/>
       <c r="L252" t="inlineStr"/>
+      <c r="M252" t="inlineStr"/>
+      <c r="N252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -7774,6 +8286,8 @@
         </is>
       </c>
       <c r="L253" t="inlineStr"/>
+      <c r="M253" t="inlineStr"/>
+      <c r="N253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -7828,6 +8342,8 @@
         </is>
       </c>
       <c r="L254" t="inlineStr"/>
+      <c r="M254" t="inlineStr"/>
+      <c r="N254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -7882,6 +8398,8 @@
         </is>
       </c>
       <c r="L255" t="inlineStr"/>
+      <c r="M255" t="inlineStr"/>
+      <c r="N255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -7936,6 +8454,8 @@
         </is>
       </c>
       <c r="L256" t="inlineStr"/>
+      <c r="M256" t="inlineStr"/>
+      <c r="N256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -7990,6 +8510,8 @@
         </is>
       </c>
       <c r="L257" t="inlineStr"/>
+      <c r="M257" t="inlineStr"/>
+      <c r="N257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -8016,6 +8538,8 @@
       <c r="J258" t="inlineStr"/>
       <c r="K258" t="inlineStr"/>
       <c r="L258" t="inlineStr"/>
+      <c r="M258" t="inlineStr"/>
+      <c r="N258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -8042,6 +8566,8 @@
       <c r="J259" t="inlineStr"/>
       <c r="K259" t="inlineStr"/>
       <c r="L259" t="inlineStr"/>
+      <c r="M259" t="inlineStr"/>
+      <c r="N259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -8068,6 +8594,8 @@
       <c r="J260" t="inlineStr"/>
       <c r="K260" t="inlineStr"/>
       <c r="L260" t="inlineStr"/>
+      <c r="M260" t="inlineStr"/>
+      <c r="N260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -8094,6 +8622,8 @@
       <c r="J261" t="inlineStr"/>
       <c r="K261" t="inlineStr"/>
       <c r="L261" t="inlineStr"/>
+      <c r="M261" t="inlineStr"/>
+      <c r="N261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -8120,6 +8650,8 @@
       <c r="J262" t="inlineStr"/>
       <c r="K262" t="inlineStr"/>
       <c r="L262" t="inlineStr"/>
+      <c r="M262" t="inlineStr"/>
+      <c r="N262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -8146,6 +8678,8 @@
       <c r="J263" t="inlineStr"/>
       <c r="K263" t="inlineStr"/>
       <c r="L263" t="inlineStr"/>
+      <c r="M263" t="inlineStr"/>
+      <c r="N263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -8172,6 +8706,8 @@
       <c r="J264" t="inlineStr"/>
       <c r="K264" t="inlineStr"/>
       <c r="L264" t="inlineStr"/>
+      <c r="M264" t="inlineStr"/>
+      <c r="N264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -8198,6 +8734,8 @@
       <c r="J265" t="inlineStr"/>
       <c r="K265" t="inlineStr"/>
       <c r="L265" t="inlineStr"/>
+      <c r="M265" t="inlineStr"/>
+      <c r="N265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -8224,6 +8762,8 @@
       <c r="J266" t="inlineStr"/>
       <c r="K266" t="inlineStr"/>
       <c r="L266" t="inlineStr"/>
+      <c r="M266" t="inlineStr"/>
+      <c r="N266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -8250,6 +8790,8 @@
       <c r="J267" t="inlineStr"/>
       <c r="K267" t="inlineStr"/>
       <c r="L267" t="inlineStr"/>
+      <c r="M267" t="inlineStr"/>
+      <c r="N267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -8276,6 +8818,8 @@
       <c r="J268" t="inlineStr"/>
       <c r="K268" t="inlineStr"/>
       <c r="L268" t="inlineStr"/>
+      <c r="M268" t="inlineStr"/>
+      <c r="N268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -8302,6 +8846,8 @@
       <c r="J269" t="inlineStr"/>
       <c r="K269" t="inlineStr"/>
       <c r="L269" t="inlineStr"/>
+      <c r="M269" t="inlineStr"/>
+      <c r="N269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -8328,6 +8874,8 @@
       <c r="J270" t="inlineStr"/>
       <c r="K270" t="inlineStr"/>
       <c r="L270" t="inlineStr"/>
+      <c r="M270" t="inlineStr"/>
+      <c r="N270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -8354,6 +8902,8 @@
       <c r="J271" t="inlineStr"/>
       <c r="K271" t="inlineStr"/>
       <c r="L271" t="inlineStr"/>
+      <c r="M271" t="inlineStr"/>
+      <c r="N271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -8380,6 +8930,8 @@
       <c r="J272" t="inlineStr"/>
       <c r="K272" t="inlineStr"/>
       <c r="L272" t="inlineStr"/>
+      <c r="M272" t="inlineStr"/>
+      <c r="N272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -8406,6 +8958,8 @@
       <c r="J273" t="inlineStr"/>
       <c r="K273" t="inlineStr"/>
       <c r="L273" t="inlineStr"/>
+      <c r="M273" t="inlineStr"/>
+      <c r="N273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -8432,6 +8986,8 @@
       <c r="J274" t="inlineStr"/>
       <c r="K274" t="inlineStr"/>
       <c r="L274" t="inlineStr"/>
+      <c r="M274" t="inlineStr"/>
+      <c r="N274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -8458,6 +9014,8 @@
       <c r="J275" t="inlineStr"/>
       <c r="K275" t="inlineStr"/>
       <c r="L275" t="inlineStr"/>
+      <c r="M275" t="inlineStr"/>
+      <c r="N275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -8484,6 +9042,8 @@
       <c r="J276" t="inlineStr"/>
       <c r="K276" t="inlineStr"/>
       <c r="L276" t="inlineStr"/>
+      <c r="M276" t="inlineStr"/>
+      <c r="N276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -8510,6 +9070,8 @@
       <c r="J277" t="inlineStr"/>
       <c r="K277" t="inlineStr"/>
       <c r="L277" t="inlineStr"/>
+      <c r="M277" t="inlineStr"/>
+      <c r="N277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -8536,6 +9098,8 @@
       <c r="J278" t="inlineStr"/>
       <c r="K278" t="inlineStr"/>
       <c r="L278" t="inlineStr"/>
+      <c r="M278" t="inlineStr"/>
+      <c r="N278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -8562,6 +9126,8 @@
       <c r="J279" t="inlineStr"/>
       <c r="K279" t="inlineStr"/>
       <c r="L279" t="inlineStr"/>
+      <c r="M279" t="inlineStr"/>
+      <c r="N279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -8588,6 +9154,8 @@
       <c r="J280" t="inlineStr"/>
       <c r="K280" t="inlineStr"/>
       <c r="L280" t="inlineStr"/>
+      <c r="M280" t="inlineStr"/>
+      <c r="N280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -8614,6 +9182,8 @@
       <c r="J281" t="inlineStr"/>
       <c r="K281" t="inlineStr"/>
       <c r="L281" t="inlineStr"/>
+      <c r="M281" t="inlineStr"/>
+      <c r="N281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -8640,6 +9210,8 @@
       <c r="J282" t="inlineStr"/>
       <c r="K282" t="inlineStr"/>
       <c r="L282" t="inlineStr"/>
+      <c r="M282" t="inlineStr"/>
+      <c r="N282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -8666,6 +9238,8 @@
       <c r="J283" t="inlineStr"/>
       <c r="K283" t="inlineStr"/>
       <c r="L283" t="inlineStr"/>
+      <c r="M283" t="inlineStr"/>
+      <c r="N283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -8692,6 +9266,8 @@
       <c r="J284" t="inlineStr"/>
       <c r="K284" t="inlineStr"/>
       <c r="L284" t="inlineStr"/>
+      <c r="M284" t="inlineStr"/>
+      <c r="N284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -8718,6 +9294,8 @@
       <c r="J285" t="inlineStr"/>
       <c r="K285" t="inlineStr"/>
       <c r="L285" t="inlineStr"/>
+      <c r="M285" t="inlineStr"/>
+      <c r="N285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -8744,6 +9322,8 @@
       <c r="J286" t="inlineStr"/>
       <c r="K286" t="inlineStr"/>
       <c r="L286" t="inlineStr"/>
+      <c r="M286" t="inlineStr"/>
+      <c r="N286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -8770,6 +9350,8 @@
       <c r="J287" t="inlineStr"/>
       <c r="K287" t="inlineStr"/>
       <c r="L287" t="inlineStr"/>
+      <c r="M287" t="inlineStr"/>
+      <c r="N287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -8796,6 +9378,8 @@
       <c r="J288" t="inlineStr"/>
       <c r="K288" t="inlineStr"/>
       <c r="L288" t="inlineStr"/>
+      <c r="M288" t="inlineStr"/>
+      <c r="N288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -8850,6 +9434,8 @@
         </is>
       </c>
       <c r="L289" t="inlineStr"/>
+      <c r="M289" t="inlineStr"/>
+      <c r="N289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -8904,6 +9490,8 @@
         </is>
       </c>
       <c r="L290" t="inlineStr"/>
+      <c r="M290" t="inlineStr"/>
+      <c r="N290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -8958,6 +9546,8 @@
         </is>
       </c>
       <c r="L291" t="inlineStr"/>
+      <c r="M291" t="inlineStr"/>
+      <c r="N291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -9012,6 +9602,8 @@
         </is>
       </c>
       <c r="L292" t="inlineStr"/>
+      <c r="M292" t="inlineStr"/>
+      <c r="N292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -9066,6 +9658,8 @@
         </is>
       </c>
       <c r="L293" t="inlineStr"/>
+      <c r="M293" t="inlineStr"/>
+      <c r="N293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -9092,6 +9686,8 @@
       <c r="J294" t="inlineStr"/>
       <c r="K294" t="inlineStr"/>
       <c r="L294" t="inlineStr"/>
+      <c r="M294" t="inlineStr"/>
+      <c r="N294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -9118,6 +9714,8 @@
       <c r="J295" t="inlineStr"/>
       <c r="K295" t="inlineStr"/>
       <c r="L295" t="inlineStr"/>
+      <c r="M295" t="inlineStr"/>
+      <c r="N295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -9144,6 +9742,8 @@
       <c r="J296" t="inlineStr"/>
       <c r="K296" t="inlineStr"/>
       <c r="L296" t="inlineStr"/>
+      <c r="M296" t="inlineStr"/>
+      <c r="N296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -9170,6 +9770,8 @@
       <c r="J297" t="inlineStr"/>
       <c r="K297" t="inlineStr"/>
       <c r="L297" t="inlineStr"/>
+      <c r="M297" t="inlineStr"/>
+      <c r="N297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -9196,6 +9798,8 @@
       <c r="J298" t="inlineStr"/>
       <c r="K298" t="inlineStr"/>
       <c r="L298" t="inlineStr"/>
+      <c r="M298" t="inlineStr"/>
+      <c r="N298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -9222,6 +9826,8 @@
       <c r="J299" t="inlineStr"/>
       <c r="K299" t="inlineStr"/>
       <c r="L299" t="inlineStr"/>
+      <c r="M299" t="inlineStr"/>
+      <c r="N299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -9248,6 +9854,8 @@
       <c r="J300" t="inlineStr"/>
       <c r="K300" t="inlineStr"/>
       <c r="L300" t="inlineStr"/>
+      <c r="M300" t="inlineStr"/>
+      <c r="N300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -9274,6 +9882,8 @@
       <c r="J301" t="inlineStr"/>
       <c r="K301" t="inlineStr"/>
       <c r="L301" t="inlineStr"/>
+      <c r="M301" t="inlineStr"/>
+      <c r="N301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -9300,6 +9910,8 @@
       <c r="J302" t="inlineStr"/>
       <c r="K302" t="inlineStr"/>
       <c r="L302" t="inlineStr"/>
+      <c r="M302" t="inlineStr"/>
+      <c r="N302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -9326,6 +9938,8 @@
       <c r="J303" t="inlineStr"/>
       <c r="K303" t="inlineStr"/>
       <c r="L303" t="inlineStr"/>
+      <c r="M303" t="inlineStr"/>
+      <c r="N303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -9352,6 +9966,8 @@
       <c r="J304" t="inlineStr"/>
       <c r="K304" t="inlineStr"/>
       <c r="L304" t="inlineStr"/>
+      <c r="M304" t="inlineStr"/>
+      <c r="N304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -9378,6 +9994,8 @@
       <c r="J305" t="inlineStr"/>
       <c r="K305" t="inlineStr"/>
       <c r="L305" t="inlineStr"/>
+      <c r="M305" t="inlineStr"/>
+      <c r="N305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -9404,6 +10022,8 @@
       <c r="J306" t="inlineStr"/>
       <c r="K306" t="inlineStr"/>
       <c r="L306" t="inlineStr"/>
+      <c r="M306" t="inlineStr"/>
+      <c r="N306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -9430,6 +10050,8 @@
       <c r="J307" t="inlineStr"/>
       <c r="K307" t="inlineStr"/>
       <c r="L307" t="inlineStr"/>
+      <c r="M307" t="inlineStr"/>
+      <c r="N307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -9456,6 +10078,8 @@
       <c r="J308" t="inlineStr"/>
       <c r="K308" t="inlineStr"/>
       <c r="L308" t="inlineStr"/>
+      <c r="M308" t="inlineStr"/>
+      <c r="N308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -9482,6 +10106,8 @@
       <c r="J309" t="inlineStr"/>
       <c r="K309" t="inlineStr"/>
       <c r="L309" t="inlineStr"/>
+      <c r="M309" t="inlineStr"/>
+      <c r="N309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -9508,6 +10134,8 @@
       <c r="J310" t="inlineStr"/>
       <c r="K310" t="inlineStr"/>
       <c r="L310" t="inlineStr"/>
+      <c r="M310" t="inlineStr"/>
+      <c r="N310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -9534,6 +10162,8 @@
       <c r="J311" t="inlineStr"/>
       <c r="K311" t="inlineStr"/>
       <c r="L311" t="inlineStr"/>
+      <c r="M311" t="inlineStr"/>
+      <c r="N311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -9560,6 +10190,8 @@
       <c r="J312" t="inlineStr"/>
       <c r="K312" t="inlineStr"/>
       <c r="L312" t="inlineStr"/>
+      <c r="M312" t="inlineStr"/>
+      <c r="N312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -9586,6 +10218,8 @@
       <c r="J313" t="inlineStr"/>
       <c r="K313" t="inlineStr"/>
       <c r="L313" t="inlineStr"/>
+      <c r="M313" t="inlineStr"/>
+      <c r="N313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -9612,6 +10246,8 @@
       <c r="J314" t="inlineStr"/>
       <c r="K314" t="inlineStr"/>
       <c r="L314" t="inlineStr"/>
+      <c r="M314" t="inlineStr"/>
+      <c r="N314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -9638,6 +10274,8 @@
       <c r="J315" t="inlineStr"/>
       <c r="K315" t="inlineStr"/>
       <c r="L315" t="inlineStr"/>
+      <c r="M315" t="inlineStr"/>
+      <c r="N315" t="inlineStr"/>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -9664,6 +10302,8 @@
       <c r="J316" t="inlineStr"/>
       <c r="K316" t="inlineStr"/>
       <c r="L316" t="inlineStr"/>
+      <c r="M316" t="inlineStr"/>
+      <c r="N316" t="inlineStr"/>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -9718,6 +10358,8 @@
         </is>
       </c>
       <c r="L317" t="inlineStr"/>
+      <c r="M317" t="inlineStr"/>
+      <c r="N317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -9772,6 +10414,8 @@
         </is>
       </c>
       <c r="L318" t="inlineStr"/>
+      <c r="M318" t="inlineStr"/>
+      <c r="N318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -9826,6 +10470,8 @@
         </is>
       </c>
       <c r="L319" t="inlineStr"/>
+      <c r="M319" t="inlineStr"/>
+      <c r="N319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -9880,6 +10526,8 @@
         </is>
       </c>
       <c r="L320" t="inlineStr"/>
+      <c r="M320" t="inlineStr"/>
+      <c r="N320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -9934,6 +10582,8 @@
         </is>
       </c>
       <c r="L321" t="inlineStr"/>
+      <c r="M321" t="inlineStr"/>
+      <c r="N321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -9960,6 +10610,8 @@
       <c r="J322" t="inlineStr"/>
       <c r="K322" t="inlineStr"/>
       <c r="L322" t="inlineStr"/>
+      <c r="M322" t="inlineStr"/>
+      <c r="N322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -9986,6 +10638,8 @@
       <c r="J323" t="inlineStr"/>
       <c r="K323" t="inlineStr"/>
       <c r="L323" t="inlineStr"/>
+      <c r="M323" t="inlineStr"/>
+      <c r="N323" t="inlineStr"/>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -10012,6 +10666,8 @@
       <c r="J324" t="inlineStr"/>
       <c r="K324" t="inlineStr"/>
       <c r="L324" t="inlineStr"/>
+      <c r="M324" t="inlineStr"/>
+      <c r="N324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -10038,6 +10694,8 @@
       <c r="J325" t="inlineStr"/>
       <c r="K325" t="inlineStr"/>
       <c r="L325" t="inlineStr"/>
+      <c r="M325" t="inlineStr"/>
+      <c r="N325" t="inlineStr"/>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -10064,6 +10722,8 @@
       <c r="J326" t="inlineStr"/>
       <c r="K326" t="inlineStr"/>
       <c r="L326" t="inlineStr"/>
+      <c r="M326" t="inlineStr"/>
+      <c r="N326" t="inlineStr"/>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -10090,6 +10750,8 @@
       <c r="J327" t="inlineStr"/>
       <c r="K327" t="inlineStr"/>
       <c r="L327" t="inlineStr"/>
+      <c r="M327" t="inlineStr"/>
+      <c r="N327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -10116,6 +10778,8 @@
       <c r="J328" t="inlineStr"/>
       <c r="K328" t="inlineStr"/>
       <c r="L328" t="inlineStr"/>
+      <c r="M328" t="inlineStr"/>
+      <c r="N328" t="inlineStr"/>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -10142,6 +10806,8 @@
       <c r="J329" t="inlineStr"/>
       <c r="K329" t="inlineStr"/>
       <c r="L329" t="inlineStr"/>
+      <c r="M329" t="inlineStr"/>
+      <c r="N329" t="inlineStr"/>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -10168,6 +10834,8 @@
       <c r="J330" t="inlineStr"/>
       <c r="K330" t="inlineStr"/>
       <c r="L330" t="inlineStr"/>
+      <c r="M330" t="inlineStr"/>
+      <c r="N330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -10194,6 +10862,8 @@
       <c r="J331" t="inlineStr"/>
       <c r="K331" t="inlineStr"/>
       <c r="L331" t="inlineStr"/>
+      <c r="M331" t="inlineStr"/>
+      <c r="N331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -10220,6 +10890,8 @@
       <c r="J332" t="inlineStr"/>
       <c r="K332" t="inlineStr"/>
       <c r="L332" t="inlineStr"/>
+      <c r="M332" t="inlineStr"/>
+      <c r="N332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -10246,6 +10918,8 @@
       <c r="J333" t="inlineStr"/>
       <c r="K333" t="inlineStr"/>
       <c r="L333" t="inlineStr"/>
+      <c r="M333" t="inlineStr"/>
+      <c r="N333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -10272,6 +10946,8 @@
       <c r="J334" t="inlineStr"/>
       <c r="K334" t="inlineStr"/>
       <c r="L334" t="inlineStr"/>
+      <c r="M334" t="inlineStr"/>
+      <c r="N334" t="inlineStr"/>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -10298,6 +10974,8 @@
       <c r="J335" t="inlineStr"/>
       <c r="K335" t="inlineStr"/>
       <c r="L335" t="inlineStr"/>
+      <c r="M335" t="inlineStr"/>
+      <c r="N335" t="inlineStr"/>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -10324,6 +11002,8 @@
       <c r="J336" t="inlineStr"/>
       <c r="K336" t="inlineStr"/>
       <c r="L336" t="inlineStr"/>
+      <c r="M336" t="inlineStr"/>
+      <c r="N336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -10350,6 +11030,8 @@
       <c r="J337" t="inlineStr"/>
       <c r="K337" t="inlineStr"/>
       <c r="L337" t="inlineStr"/>
+      <c r="M337" t="inlineStr"/>
+      <c r="N337" t="inlineStr"/>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -10376,6 +11058,8 @@
       <c r="J338" t="inlineStr"/>
       <c r="K338" t="inlineStr"/>
       <c r="L338" t="inlineStr"/>
+      <c r="M338" t="inlineStr"/>
+      <c r="N338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -10402,6 +11086,8 @@
       <c r="J339" t="inlineStr"/>
       <c r="K339" t="inlineStr"/>
       <c r="L339" t="inlineStr"/>
+      <c r="M339" t="inlineStr"/>
+      <c r="N339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -10428,6 +11114,8 @@
       <c r="J340" t="inlineStr"/>
       <c r="K340" t="inlineStr"/>
       <c r="L340" t="inlineStr"/>
+      <c r="M340" t="inlineStr"/>
+      <c r="N340" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -10454,6 +11142,8 @@
       <c r="J341" t="inlineStr"/>
       <c r="K341" t="inlineStr"/>
       <c r="L341" t="inlineStr"/>
+      <c r="M341" t="inlineStr"/>
+      <c r="N341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -10480,6 +11170,8 @@
       <c r="J342" t="inlineStr"/>
       <c r="K342" t="inlineStr"/>
       <c r="L342" t="inlineStr"/>
+      <c r="M342" t="inlineStr"/>
+      <c r="N342" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -10506,6 +11198,8 @@
       <c r="J343" t="inlineStr"/>
       <c r="K343" t="inlineStr"/>
       <c r="L343" t="inlineStr"/>
+      <c r="M343" t="inlineStr"/>
+      <c r="N343" t="inlineStr"/>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -10532,6 +11226,8 @@
       <c r="J344" t="inlineStr"/>
       <c r="K344" t="inlineStr"/>
       <c r="L344" t="inlineStr"/>
+      <c r="M344" t="inlineStr"/>
+      <c r="N344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -10558,6 +11254,8 @@
       <c r="J345" t="inlineStr"/>
       <c r="K345" t="inlineStr"/>
       <c r="L345" t="inlineStr"/>
+      <c r="M345" t="inlineStr"/>
+      <c r="N345" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -10584,6 +11282,8 @@
       <c r="J346" t="inlineStr"/>
       <c r="K346" t="inlineStr"/>
       <c r="L346" t="inlineStr"/>
+      <c r="M346" t="inlineStr"/>
+      <c r="N346" t="inlineStr"/>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -10610,6 +11310,8 @@
       <c r="J347" t="inlineStr"/>
       <c r="K347" t="inlineStr"/>
       <c r="L347" t="inlineStr"/>
+      <c r="M347" t="inlineStr"/>
+      <c r="N347" t="inlineStr"/>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -10664,6 +11366,8 @@
         </is>
       </c>
       <c r="L348" t="inlineStr"/>
+      <c r="M348" t="inlineStr"/>
+      <c r="N348" t="inlineStr"/>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -10718,6 +11422,8 @@
         </is>
       </c>
       <c r="L349" t="inlineStr"/>
+      <c r="M349" t="inlineStr"/>
+      <c r="N349" t="inlineStr"/>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -10772,6 +11478,8 @@
         </is>
       </c>
       <c r="L350" t="inlineStr"/>
+      <c r="M350" t="inlineStr"/>
+      <c r="N350" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -10826,6 +11534,8 @@
         </is>
       </c>
       <c r="L351" t="inlineStr"/>
+      <c r="M351" t="inlineStr"/>
+      <c r="N351" t="inlineStr"/>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -10880,6 +11590,8 @@
         </is>
       </c>
       <c r="L352" t="inlineStr"/>
+      <c r="M352" t="inlineStr"/>
+      <c r="N352" t="inlineStr"/>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -10906,6 +11618,8 @@
       <c r="J353" t="inlineStr"/>
       <c r="K353" t="inlineStr"/>
       <c r="L353" t="inlineStr"/>
+      <c r="M353" t="inlineStr"/>
+      <c r="N353" t="inlineStr"/>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -10960,6 +11674,8 @@
         </is>
       </c>
       <c r="L354" t="inlineStr"/>
+      <c r="M354" t="inlineStr"/>
+      <c r="N354" t="inlineStr"/>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -11014,6 +11730,8 @@
         </is>
       </c>
       <c r="L355" t="inlineStr"/>
+      <c r="M355" t="inlineStr"/>
+      <c r="N355" t="inlineStr"/>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -11068,6 +11786,8 @@
         </is>
       </c>
       <c r="L356" t="inlineStr"/>
+      <c r="M356" t="inlineStr"/>
+      <c r="N356" t="inlineStr"/>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -11122,6 +11842,8 @@
         </is>
       </c>
       <c r="L357" t="inlineStr"/>
+      <c r="M357" t="inlineStr"/>
+      <c r="N357" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -11176,6 +11898,8 @@
         </is>
       </c>
       <c r="L358" t="inlineStr"/>
+      <c r="M358" t="inlineStr"/>
+      <c r="N358" t="inlineStr"/>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -11206,6 +11930,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M359" t="inlineStr"/>
+      <c r="N359" t="inlineStr"/>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -11236,6 +11962,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M360" t="inlineStr"/>
+      <c r="N360" t="inlineStr"/>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -11266,6 +11994,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M361" t="inlineStr"/>
+      <c r="N361" t="inlineStr"/>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -11296,6 +12026,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M362" t="inlineStr"/>
+      <c r="N362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -11326,6 +12058,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M363" t="inlineStr"/>
+      <c r="N363" t="inlineStr"/>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -11356,6 +12090,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M364" t="inlineStr"/>
+      <c r="N364" t="inlineStr"/>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -11386,6 +12122,8 @@
           <t>{Timestamp('2023-05-02 00:00:00')}</t>
         </is>
       </c>
+      <c r="M365" t="inlineStr"/>
+      <c r="N365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -11416,6 +12154,8 @@
           <t>{Timestamp('2023-05-02 00:00:00')}</t>
         </is>
       </c>
+      <c r="M366" t="inlineStr"/>
+      <c r="N366" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -11446,6 +12186,8 @@
           <t>{Timestamp('2023-05-02 00:00:00')}</t>
         </is>
       </c>
+      <c r="M367" t="inlineStr"/>
+      <c r="N367" t="inlineStr"/>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -11476,6 +12218,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M368" t="inlineStr"/>
+      <c r="N368" t="inlineStr"/>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -11506,6 +12250,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M369" t="inlineStr"/>
+      <c r="N369" t="inlineStr"/>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -11536,6 +12282,8 @@
           <t>{Timestamp('2023-05-02 00:00:00')}</t>
         </is>
       </c>
+      <c r="M370" t="inlineStr"/>
+      <c r="N370" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -11566,6 +12314,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M371" t="inlineStr"/>
+      <c r="N371" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -11596,6 +12346,8 @@
           <t>{Timestamp('2023-05-02 00:00:00')}</t>
         </is>
       </c>
+      <c r="M372" t="inlineStr"/>
+      <c r="N372" t="inlineStr"/>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -11626,6 +12378,8 @@
           <t>{Timestamp('2023-05-02 00:00:00')}</t>
         </is>
       </c>
+      <c r="M373" t="inlineStr"/>
+      <c r="N373" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -11656,6 +12410,8 @@
           <t>{Timestamp('2023-05-02 00:00:00')}</t>
         </is>
       </c>
+      <c r="M374" t="inlineStr"/>
+      <c r="N374" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -11686,6 +12442,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M375" t="inlineStr"/>
+      <c r="N375" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -11716,6 +12474,8 @@
           <t>{Timestamp('2023-05-02 00:00:00')}</t>
         </is>
       </c>
+      <c r="M376" t="inlineStr"/>
+      <c r="N376" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -11746,6 +12506,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M377" t="inlineStr"/>
+      <c r="N377" t="inlineStr"/>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -11776,6 +12538,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M378" t="inlineStr"/>
+      <c r="N378" t="inlineStr"/>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -11806,6 +12570,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M379" t="inlineStr"/>
+      <c r="N379" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -11836,6 +12602,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M380" t="inlineStr"/>
+      <c r="N380" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -11866,6 +12634,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M381" t="inlineStr"/>
+      <c r="N381" t="inlineStr"/>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -11896,6 +12666,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M382" t="inlineStr"/>
+      <c r="N382" t="inlineStr"/>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -11926,6 +12698,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M383" t="inlineStr"/>
+      <c r="N383" t="inlineStr"/>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -11956,6 +12730,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M384" t="inlineStr"/>
+      <c r="N384" t="inlineStr"/>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -11986,6 +12762,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M385" t="inlineStr"/>
+      <c r="N385" t="inlineStr"/>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -12016,6 +12794,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M386" t="inlineStr"/>
+      <c r="N386" t="inlineStr"/>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -12046,6 +12826,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M387" t="inlineStr"/>
+      <c r="N387" t="inlineStr"/>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -12076,6 +12858,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M388" t="inlineStr"/>
+      <c r="N388" t="inlineStr"/>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -12106,6 +12890,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M389" t="inlineStr"/>
+      <c r="N389" t="inlineStr"/>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -12136,6 +12922,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M390" t="inlineStr"/>
+      <c r="N390" t="inlineStr"/>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -12162,6 +12950,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M391" t="inlineStr"/>
+      <c r="N391" t="inlineStr"/>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -12188,6 +12978,8 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M392" t="inlineStr"/>
+      <c r="N392" t="inlineStr"/>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -12214,6 +13006,660 @@
           <t>{Timestamp('2023-05-03 00:00:00')}</t>
         </is>
       </c>
+      <c r="M393" t="inlineStr"/>
+      <c r="N393" t="inlineStr"/>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>67-179</t>
+        </is>
+      </c>
+      <c r="B394" t="n">
+        <v>67</v>
+      </c>
+      <c r="C394" t="n">
+        <v>179</v>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>Mauerwerk</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr"/>
+      <c r="F394" t="inlineStr"/>
+      <c r="G394" t="inlineStr"/>
+      <c r="H394" t="inlineStr"/>
+      <c r="I394" t="inlineStr"/>
+      <c r="J394" t="inlineStr"/>
+      <c r="K394" t="inlineStr"/>
+      <c r="L394" t="inlineStr"/>
+      <c r="M394" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="N394" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>65-180</t>
+        </is>
+      </c>
+      <c r="B395" t="n">
+        <v>65</v>
+      </c>
+      <c r="C395" t="n">
+        <v>180</v>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>Beton</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr"/>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="H395" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="I395" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="J395" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="K395" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+      <c r="L395" t="inlineStr"/>
+      <c r="M395" t="inlineStr"/>
+      <c r="N395" t="inlineStr"/>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>67-180</t>
+        </is>
+      </c>
+      <c r="B396" t="n">
+        <v>67</v>
+      </c>
+      <c r="C396" t="n">
+        <v>180</v>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>Mauerwerk</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr"/>
+      <c r="F396" t="inlineStr"/>
+      <c r="G396" t="inlineStr"/>
+      <c r="H396" t="inlineStr"/>
+      <c r="I396" t="inlineStr"/>
+      <c r="J396" t="inlineStr"/>
+      <c r="K396" t="inlineStr"/>
+      <c r="L396" t="inlineStr"/>
+      <c r="M396" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="N396" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>65-181</t>
+        </is>
+      </c>
+      <c r="B397" t="n">
+        <v>65</v>
+      </c>
+      <c r="C397" t="n">
+        <v>181</v>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>Beton</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr"/>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="J397" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="K397" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+      <c r="L397" t="inlineStr"/>
+      <c r="M397" t="inlineStr"/>
+      <c r="N397" t="inlineStr"/>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>67-181</t>
+        </is>
+      </c>
+      <c r="B398" t="n">
+        <v>67</v>
+      </c>
+      <c r="C398" t="n">
+        <v>181</v>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>Mauerwerk</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr"/>
+      <c r="F398" t="inlineStr"/>
+      <c r="G398" t="inlineStr"/>
+      <c r="H398" t="inlineStr"/>
+      <c r="I398" t="inlineStr"/>
+      <c r="J398" t="inlineStr"/>
+      <c r="K398" t="inlineStr"/>
+      <c r="L398" t="inlineStr"/>
+      <c r="M398" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="N398" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>65-182</t>
+        </is>
+      </c>
+      <c r="B399" t="n">
+        <v>65</v>
+      </c>
+      <c r="C399" t="n">
+        <v>182</v>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>Beton</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr"/>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="H399" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="J399" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="K399" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+      <c r="L399" t="inlineStr"/>
+      <c r="M399" t="inlineStr"/>
+      <c r="N399" t="inlineStr"/>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>67-182</t>
+        </is>
+      </c>
+      <c r="B400" t="n">
+        <v>67</v>
+      </c>
+      <c r="C400" t="n">
+        <v>182</v>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>Mauerwerk</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr"/>
+      <c r="F400" t="inlineStr"/>
+      <c r="G400" t="inlineStr"/>
+      <c r="H400" t="inlineStr"/>
+      <c r="I400" t="inlineStr"/>
+      <c r="J400" t="inlineStr"/>
+      <c r="K400" t="inlineStr"/>
+      <c r="L400" t="inlineStr"/>
+      <c r="M400" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="N400" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>65-183</t>
+        </is>
+      </c>
+      <c r="B401" t="n">
+        <v>65</v>
+      </c>
+      <c r="C401" t="n">
+        <v>183</v>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>Beton</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr"/>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="H401" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="J401" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="K401" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+      <c r="L401" t="inlineStr"/>
+      <c r="M401" t="inlineStr"/>
+      <c r="N401" t="inlineStr"/>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>67-183</t>
+        </is>
+      </c>
+      <c r="B402" t="n">
+        <v>67</v>
+      </c>
+      <c r="C402" t="n">
+        <v>183</v>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>Mauerwerk</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr"/>
+      <c r="F402" t="inlineStr"/>
+      <c r="G402" t="inlineStr"/>
+      <c r="H402" t="inlineStr"/>
+      <c r="I402" t="inlineStr"/>
+      <c r="J402" t="inlineStr"/>
+      <c r="K402" t="inlineStr"/>
+      <c r="L402" t="inlineStr"/>
+      <c r="M402" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="N402" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>65-184</t>
+        </is>
+      </c>
+      <c r="B403" t="n">
+        <v>65</v>
+      </c>
+      <c r="C403" t="n">
+        <v>184</v>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>Beton</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr"/>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="H403" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="J403" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="K403" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+      <c r="L403" t="inlineStr"/>
+      <c r="M403" t="inlineStr"/>
+      <c r="N403" t="inlineStr"/>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>67-184</t>
+        </is>
+      </c>
+      <c r="B404" t="n">
+        <v>67</v>
+      </c>
+      <c r="C404" t="n">
+        <v>184</v>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>Mauerwerk</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr"/>
+      <c r="F404" t="inlineStr"/>
+      <c r="G404" t="inlineStr"/>
+      <c r="H404" t="inlineStr"/>
+      <c r="I404" t="inlineStr"/>
+      <c r="J404" t="inlineStr"/>
+      <c r="K404" t="inlineStr"/>
+      <c r="L404" t="inlineStr"/>
+      <c r="M404" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="N404" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>65-185</t>
+        </is>
+      </c>
+      <c r="B405" t="n">
+        <v>65</v>
+      </c>
+      <c r="C405" t="n">
+        <v>185</v>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>Beton</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr"/>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="H405" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="J405" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="K405" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+      <c r="L405" t="inlineStr"/>
+      <c r="M405" t="inlineStr"/>
+      <c r="N405" t="inlineStr"/>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>67-185</t>
+        </is>
+      </c>
+      <c r="B406" t="n">
+        <v>67</v>
+      </c>
+      <c r="C406" t="n">
+        <v>185</v>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>Mauerwerk</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr"/>
+      <c r="F406" t="inlineStr"/>
+      <c r="G406" t="inlineStr"/>
+      <c r="H406" t="inlineStr"/>
+      <c r="I406" t="inlineStr"/>
+      <c r="J406" t="inlineStr"/>
+      <c r="K406" t="inlineStr"/>
+      <c r="L406" t="inlineStr"/>
+      <c r="M406" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="N406" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>65-186</t>
+        </is>
+      </c>
+      <c r="B407" t="n">
+        <v>65</v>
+      </c>
+      <c r="C407" t="n">
+        <v>186</v>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>Beton</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr"/>
+      <c r="F407" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="G407" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="H407" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="I407" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="J407" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="K407" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
+      <c r="L407" t="inlineStr"/>
+      <c r="M407" t="inlineStr"/>
+      <c r="N407" t="inlineStr"/>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>67-186</t>
+        </is>
+      </c>
+      <c r="B408" t="n">
+        <v>67</v>
+      </c>
+      <c r="C408" t="n">
+        <v>186</v>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>Mauerwerk</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr"/>
+      <c r="F408" t="inlineStr"/>
+      <c r="G408" t="inlineStr"/>
+      <c r="H408" t="inlineStr"/>
+      <c r="I408" t="inlineStr"/>
+      <c r="J408" t="inlineStr"/>
+      <c r="K408" t="inlineStr"/>
+      <c r="L408" t="inlineStr"/>
+      <c r="M408" t="inlineStr">
+        <is>
+          <t>set()</t>
+        </is>
+      </c>
+      <c r="N408" t="inlineStr">
+        <is>
+          <t>{Timestamp('2023-06-21 00:00:00')}</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>